<commit_message>
cập nhật tối 5/6/2025
</commit_message>
<xml_diff>
--- a/Dự án cây xanh/WBS_QuanLyDuAnCayXanh.xlsx
+++ b/Dự án cây xanh/WBS_QuanLyDuAnCayXanh.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\InternTester\Project\Dự án cây xanh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE140A07-55F5-47FB-87B1-F8EFD7C9ACB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12500B2A-0B9A-4CBF-8D98-96658A45D6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1540,22 +1540,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF7F7F7F"/>
-          <bgColor rgb="FF7F7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FF0070C0"/>
           <bgColor rgb="FF0070C0"/>
         </patternFill>
@@ -1573,122 +1557,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7F7F7F"/>
-          <bgColor rgb="FF7F7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7F7F7F"/>
-          <bgColor rgb="FF7F7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7F7F7F"/>
-          <bgColor rgb="FF7F7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7F7F7F"/>
-          <bgColor rgb="FF7F7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7F7F7F"/>
-          <bgColor rgb="FF7F7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7F7F7F"/>
-          <bgColor rgb="FF7F7F7F"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1726,25 +1594,8 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7F7F7F"/>
-          <bgColor rgb="FF7F7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF0070C0"/>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1766,9 +1617,8 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7F7F7F"/>
-          <bgColor rgb="FF7F7F7F"/>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1790,41 +1640,8 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7F7F7F"/>
-          <bgColor rgb="FF7F7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7F7F7F"/>
-          <bgColor rgb="FF7F7F7F"/>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1902,38 +1719,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF7F7F7F"/>
-          <bgColor rgb="FF7F7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7F7F7F"/>
-          <bgColor rgb="FF7F7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FF0070C0"/>
           <bgColor rgb="FF0070C0"/>
         </patternFill>
@@ -1960,6 +1745,22 @@
         <patternFill patternType="solid">
           <fgColor rgb="FF7F7F7F"/>
           <bgColor rgb="FF7F7F7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7F7F7F"/>
+          <bgColor rgb="FF7F7F7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF0070C0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2068,6 +1869,205 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7F7F7F"/>
+          <bgColor rgb="FF7F7F7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7F7F7F"/>
+          <bgColor rgb="FF7F7F7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7F7F7F"/>
+          <bgColor rgb="FF7F7F7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7F7F7F"/>
+          <bgColor rgb="FF7F7F7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7F7F7F"/>
+          <bgColor rgb="FF7F7F7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7F7F7F"/>
+          <bgColor rgb="FF7F7F7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7F7F7F"/>
+          <bgColor rgb="FF7F7F7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7F7F7F"/>
+          <bgColor rgb="FF7F7F7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7F7F7F"/>
+          <bgColor rgb="FF7F7F7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7F7F7F"/>
+          <bgColor rgb="FF7F7F7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7F7F7F"/>
+          <bgColor rgb="FF7F7F7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7F7F7F"/>
+          <bgColor rgb="FF7F7F7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.34998626667073579"/>
         </patternFill>
@@ -2135,9 +2135,8 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7F7F7F"/>
-          <bgColor rgb="FF7F7F7F"/>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2151,8 +2150,9 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7F7F7F"/>
+          <bgColor rgb="FF7F7F7F"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2181,29 +2181,6 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7F7F7F"/>
-          <bgColor rgb="FF7F7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.34998626667073579"/>
         </patternFill>
@@ -2222,236 +2199,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FF7F7F7F"/>
           <bgColor rgb="FF7F7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7F7F7F"/>
-          <bgColor rgb="FF7F7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7F7F7F"/>
-          <bgColor rgb="FF7F7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7F7F7F"/>
-          <bgColor rgb="FF7F7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7F7F7F"/>
-          <bgColor rgb="FF7F7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7F7F7F"/>
-          <bgColor rgb="FF7F7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7F7F7F"/>
-          <bgColor rgb="FF7F7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7F7F7F"/>
-          <bgColor rgb="FF7F7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7F7F7F"/>
-          <bgColor rgb="FF7F7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7F7F7F"/>
-          <bgColor rgb="FF7F7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7F7F7F"/>
-          <bgColor rgb="FF7F7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF0070C0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2557,8 +2304,116 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7F7F7F"/>
+          <bgColor rgb="FF7F7F7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7F7F7F"/>
+          <bgColor rgb="FF7F7F7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7F7F7F"/>
+          <bgColor rgb="FF7F7F7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7F7F7F"/>
+          <bgColor rgb="FF7F7F7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7F7F7F"/>
+          <bgColor rgb="FF7F7F7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF0070C0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2587,14 +2442,6 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.34998626667073579"/>
         </patternFill>
@@ -2603,23 +2450,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF7F7F7F"/>
-          <bgColor rgb="FF7F7F7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FF0070C0"/>
           <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2694,6 +2526,75 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7F7F7F"/>
+          <bgColor rgb="FF7F7F7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7F7F7F"/>
+          <bgColor rgb="FF7F7F7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7F7F7F"/>
+          <bgColor rgb="FF7F7F7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF7F7F7F"/>
           <bgColor rgb="FF7F7F7F"/>
@@ -2712,6 +2613,105 @@
         <patternFill patternType="solid">
           <fgColor rgb="FF0070C0"/>
           <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7F7F7F"/>
+          <bgColor rgb="FF7F7F7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7F7F7F"/>
+          <bgColor rgb="FF7F7F7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7F7F7F"/>
+          <bgColor rgb="FF7F7F7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7F7F7F"/>
+          <bgColor rgb="FF7F7F7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2888,16 +2888,16 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF0070C0"/>
+          <fgColor rgb="FF7F7F7F"/>
+          <bgColor rgb="FF7F7F7F"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF7F7F7F"/>
-          <bgColor rgb="FF7F7F7F"/>
+          <fgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF0070C0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3155,8 +3155,8 @@
   <dimension ref="A1:BN170"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M27" sqref="M27"/>
+      <pane ySplit="7" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5515,7 +5515,7 @@
         <v>1</v>
       </c>
       <c r="H25" s="36">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="I25" s="37">
         <f t="shared" si="3"/>
@@ -5601,7 +5601,7 @@
         <v>1</v>
       </c>
       <c r="H26" s="36">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="I26" s="37">
         <f t="shared" si="3"/>
@@ -5686,7 +5686,9 @@
       <c r="G27" s="35">
         <v>1</v>
       </c>
-      <c r="H27" s="36"/>
+      <c r="H27" s="36">
+        <v>1</v>
+      </c>
       <c r="I27" s="37">
         <f t="shared" si="3"/>
         <v>1</v>
@@ -5770,7 +5772,9 @@
       <c r="G28" s="35">
         <v>1</v>
       </c>
-      <c r="H28" s="36"/>
+      <c r="H28" s="36">
+        <v>1</v>
+      </c>
       <c r="I28" s="37">
         <f t="shared" si="3"/>
         <v>1</v>
@@ -5853,7 +5857,9 @@
       <c r="G29" s="35">
         <v>1</v>
       </c>
-      <c r="H29" s="36"/>
+      <c r="H29" s="36">
+        <v>1</v>
+      </c>
       <c r="I29" s="37">
         <f t="shared" si="3"/>
         <v>1</v>
@@ -5937,7 +5943,9 @@
       <c r="G30" s="35">
         <v>1</v>
       </c>
-      <c r="H30" s="36"/>
+      <c r="H30" s="36">
+        <v>1</v>
+      </c>
       <c r="I30" s="37">
         <f t="shared" si="3"/>
         <v>1</v>
@@ -17715,11 +17723,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:BN29 Y30:BN30 K30:V34 X31:BN34 K35:BN35 K36:V58 X36:BN58 K59:BN59 K60:V170 X60:BN170 W92:W93 W102">
-    <cfRule type="expression" dxfId="175" priority="153">
+    <cfRule type="expression" dxfId="175" priority="154">
+      <formula>AND(NOT(ISBLANK($E8)),$E8&lt;=K$6,$F8&gt;=K$6,WEEKDAY(K$6,2)&lt;=5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="174" priority="153">
       <formula>AND($E8&lt;=K$6,ROUNDDOWN(($F8-$E8+1)*$H8,0)+$E8-1&gt;=K$6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="174" priority="154">
-      <formula>AND(NOT(ISBLANK($E8)),$E8&lt;=K$6,$F8&gt;=K$6,WEEKDAY(K$6,2)&lt;=5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W30:W31">
@@ -17825,25 +17833,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W54">
-    <cfRule type="expression" dxfId="151" priority="3951">
-      <formula>AND(NOT(ISBLANK($E49)),$E49&lt;=W$6,$F49&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="150" priority="3949">
+    <cfRule type="expression" dxfId="151" priority="3949">
       <formula>AND(NOT(ISBLANK($E163)),$E163&lt;=X$6,$F163&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="149" priority="3950">
+    <cfRule type="expression" dxfId="150" priority="3950">
       <formula>AND($E49&lt;=W$6,ROUNDDOWN(($F49-$E49+1)*$H49,0)+$E49-1&gt;=W$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="149" priority="3951">
+      <formula>AND(NOT(ISBLANK($E49)),$E49&lt;=W$6,$F49&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W55">
-    <cfRule type="expression" dxfId="148" priority="3954">
-      <formula>AND(NOT(ISBLANK($E49)),$E49&lt;=W$6,$F49&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
+    <cfRule type="expression" dxfId="148" priority="3952">
+      <formula>AND(NOT(ISBLANK($E163)),$E163&lt;=X$6,$F163&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="147" priority="3953">
       <formula>AND($E49&lt;=W$6,ROUNDDOWN(($F49-$E49+1)*$H49,0)+$E49-1&gt;=W$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="146" priority="3952">
-      <formula>AND(NOT(ISBLANK($E163)),$E163&lt;=X$6,$F163&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
+    <cfRule type="expression" dxfId="146" priority="3954">
+      <formula>AND(NOT(ISBLANK($E49)),$E49&lt;=W$6,$F49&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W56">
@@ -17852,36 +17860,36 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W57">
-    <cfRule type="expression" dxfId="144" priority="3958">
-      <formula>AND(NOT(ISBLANK($E49)),$E49&lt;=W$6,$F49&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
+    <cfRule type="expression" dxfId="144" priority="3956">
+      <formula>AND(NOT(ISBLANK($E163)),$E163&lt;=X$6,$F163&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="143" priority="3957">
       <formula>AND($E49&lt;=W$6,ROUNDDOWN(($F49-$E49+1)*$H49,0)+$E49-1&gt;=W$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="142" priority="3956">
-      <formula>AND(NOT(ISBLANK($E163)),$E163&lt;=X$6,$F163&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
+    <cfRule type="expression" dxfId="142" priority="3958">
+      <formula>AND(NOT(ISBLANK($E49)),$E49&lt;=W$6,$F49&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W58">
-    <cfRule type="expression" dxfId="141" priority="3960">
+    <cfRule type="expression" dxfId="141" priority="3959">
+      <formula>AND(NOT(ISBLANK($E163)),$E163&lt;=X$6,$F163&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="140" priority="3960">
       <formula>AND($E49&lt;=W$6,ROUNDDOWN(($F49-$E49+1)*$H49,0)+$E49-1&gt;=W$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="140" priority="3961">
+    <cfRule type="expression" dxfId="139" priority="3961">
       <formula>AND(NOT(ISBLANK($E49)),$E49&lt;=W$6,$F49&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="139" priority="3959">
-      <formula>AND(NOT(ISBLANK($E163)),$E163&lt;=X$6,$F163&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W60">
     <cfRule type="expression" dxfId="138" priority="3964">
       <formula>AND(NOT(ISBLANK($E49)),$E49&lt;=W$6,$F49&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="137" priority="3963">
+    <cfRule type="expression" dxfId="137" priority="3962">
+      <formula>AND(NOT(ISBLANK($E163)),$E163&lt;=X$6,$F163&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="136" priority="3963">
       <formula>AND($E49&lt;=W$6,ROUNDDOWN(($F49-$E49+1)*$H49,0)+$E49-1&gt;=W$6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="136" priority="3962">
-      <formula>AND(NOT(ISBLANK($E163)),$E163&lt;=X$6,$F163&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W61">
@@ -17896,88 +17904,88 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W62">
-    <cfRule type="expression" dxfId="132" priority="3969">
+    <cfRule type="expression" dxfId="132" priority="3970">
+      <formula>AND(NOT(ISBLANK($E49)),$E49&lt;=W$6,$F49&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="131" priority="3969">
       <formula>AND($E49&lt;=W$6,ROUNDDOWN(($F49-$E49+1)*$H49,0)+$E49-1&gt;=W$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="131" priority="3968">
+    <cfRule type="expression" dxfId="130" priority="3968">
       <formula>AND(NOT(ISBLANK($E163)),$E163&lt;=X$6,$F163&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="130" priority="3970">
-      <formula>AND(NOT(ISBLANK($E49)),$E49&lt;=W$6,$F49&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W63">
-    <cfRule type="expression" dxfId="129" priority="3971">
-      <formula>AND(NOT(ISBLANK($E163)),$E163&lt;=X$6,$F163&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
+    <cfRule type="expression" dxfId="129" priority="3973">
+      <formula>AND(NOT(ISBLANK($E49)),$E49&lt;=W$6,$F49&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="128" priority="3972">
       <formula>AND($E49&lt;=W$6,ROUNDDOWN(($F49-$E49+1)*$H49,0)+$E49-1&gt;=W$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="127" priority="3973">
-      <formula>AND(NOT(ISBLANK($E49)),$E49&lt;=W$6,$F49&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
+    <cfRule type="expression" dxfId="127" priority="3971">
+      <formula>AND(NOT(ISBLANK($E163)),$E163&lt;=X$6,$F163&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W64">
-    <cfRule type="expression" dxfId="126" priority="3974">
-      <formula>AND(NOT(ISBLANK($E163)),$E163&lt;=X$6,$F163&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
+    <cfRule type="expression" dxfId="126" priority="3976">
+      <formula>AND(NOT(ISBLANK($E49)),$E49&lt;=W$6,$F49&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="125" priority="3975">
       <formula>AND($E49&lt;=W$6,ROUNDDOWN(($F49-$E49+1)*$H49,0)+$E49-1&gt;=W$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="3976">
-      <formula>AND(NOT(ISBLANK($E49)),$E49&lt;=W$6,$F49&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
+    <cfRule type="expression" dxfId="124" priority="3974">
+      <formula>AND(NOT(ISBLANK($E163)),$E163&lt;=X$6,$F163&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W65:W66">
-    <cfRule type="expression" dxfId="123" priority="3977">
-      <formula>AND($E49&lt;=W$6,ROUNDDOWN(($F49-$E49+1)*$H49,0)+$E49-1&gt;=W$6)</formula>
+    <cfRule type="expression" dxfId="123" priority="3979">
+      <formula>AND(NOT(ISBLANK($E163)),$E163&lt;=X$6,$F163&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="122" priority="3978">
       <formula>AND(NOT(ISBLANK($E49)),$E49&lt;=W$6,$F49&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="121" priority="3979">
-      <formula>AND(NOT(ISBLANK($E163)),$E163&lt;=X$6,$F163&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
+    <cfRule type="expression" dxfId="121" priority="3977">
+      <formula>AND($E49&lt;=W$6,ROUNDDOWN(($F49-$E49+1)*$H49,0)+$E49-1&gt;=W$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W67">
-    <cfRule type="expression" dxfId="120" priority="3982">
-      <formula>AND(NOT(ISBLANK($E50)),$E50&lt;=W$6,$F50&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="119" priority="3980">
+    <cfRule type="expression" dxfId="120" priority="3980">
       <formula>AND(NOT(ISBLANK($E164)),$E164&lt;=X$6,$F164&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="3981">
+    <cfRule type="expression" dxfId="119" priority="3981">
       <formula>AND($E50&lt;=W$6,ROUNDDOWN(($F50-$E50+1)*$H50,0)+$E50-1&gt;=W$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="118" priority="3982">
+      <formula>AND(NOT(ISBLANK($E50)),$E50&lt;=W$6,$F50&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W68">
     <cfRule type="expression" dxfId="117" priority="3985">
       <formula>AND(NOT(ISBLANK($E50)),$E50&lt;=W$6,$F50&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="3984">
+    <cfRule type="expression" dxfId="116" priority="3983">
+      <formula>AND(NOT(ISBLANK($E164)),$E164&lt;=X$6,$F164&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="115" priority="3984">
       <formula>AND($E50&lt;=W$6,ROUNDDOWN(($F50-$E50+1)*$H50,0)+$E50-1&gt;=W$6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="115" priority="3983">
-      <formula>AND(NOT(ISBLANK($E164)),$E164&lt;=X$6,$F164&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W69">
-    <cfRule type="expression" dxfId="114" priority="3988">
-      <formula>AND(NOT(ISBLANK($E50)),$E50&lt;=W$6,$F50&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
+    <cfRule type="expression" dxfId="114" priority="3986">
+      <formula>AND(NOT(ISBLANK($E164)),$E164&lt;=X$6,$F164&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="113" priority="3987">
       <formula>AND($E50&lt;=W$6,ROUNDDOWN(($F50-$E50+1)*$H50,0)+$E50-1&gt;=W$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="3986">
-      <formula>AND(NOT(ISBLANK($E164)),$E164&lt;=X$6,$F164&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
+    <cfRule type="expression" dxfId="112" priority="3988">
+      <formula>AND(NOT(ISBLANK($E50)),$E50&lt;=W$6,$F50&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W70">
-    <cfRule type="expression" dxfId="111" priority="3991">
+    <cfRule type="expression" dxfId="111" priority="3990">
+      <formula>AND($E50&lt;=W$6,ROUNDDOWN(($F50-$E50+1)*$H50,0)+$E50-1&gt;=W$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="110" priority="3991">
       <formula>AND(NOT(ISBLANK($E50)),$E50&lt;=W$6,$F50&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="110" priority="3990">
-      <formula>AND($E50&lt;=W$6,ROUNDDOWN(($F50-$E50+1)*$H50,0)+$E50-1&gt;=W$6)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="109" priority="3989">
       <formula>AND(NOT(ISBLANK($E164)),$E164&lt;=X$6,$F164&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
@@ -17987,44 +17995,44 @@
     <cfRule type="expression" dxfId="108" priority="3993">
       <formula>AND($E50&lt;=W$6,ROUNDDOWN(($F50-$E50+1)*$H50,0)+$E50-1&gt;=W$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="3992">
+    <cfRule type="expression" dxfId="107" priority="3994">
+      <formula>AND(NOT(ISBLANK($E50)),$E50&lt;=W$6,$F50&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="106" priority="3992">
       <formula>AND(NOT(ISBLANK($E164)),$E164&lt;=X$6,$F164&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="106" priority="3994">
-      <formula>AND(NOT(ISBLANK($E50)),$E50&lt;=W$6,$F50&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W72:W73">
-    <cfRule type="expression" dxfId="105" priority="3997">
-      <formula>AND(NOT(ISBLANK($E50)),$E50&lt;=W$6,$F50&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
+    <cfRule type="expression" dxfId="105" priority="3995">
+      <formula>AND(NOT(ISBLANK($E164)),$E164&lt;=X$6,$F164&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="104" priority="3996">
       <formula>AND($E50&lt;=W$6,ROUNDDOWN(($F50-$E50+1)*$H50,0)+$E50-1&gt;=W$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="3995">
-      <formula>AND(NOT(ISBLANK($E164)),$E164&lt;=X$6,$F164&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
+    <cfRule type="expression" dxfId="103" priority="3997">
+      <formula>AND(NOT(ISBLANK($E50)),$E50&lt;=W$6,$F50&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W74">
-    <cfRule type="expression" dxfId="102" priority="4000">
-      <formula>AND(NOT(ISBLANK($E51)),$E51&lt;=W$6,$F51&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
+    <cfRule type="expression" dxfId="102" priority="3998">
+      <formula>AND(NOT(ISBLANK($E165)),$E165&lt;=X$6,$F165&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="101" priority="3999">
       <formula>AND($E51&lt;=W$6,ROUNDDOWN(($F51-$E51+1)*$H51,0)+$E51-1&gt;=W$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="3998">
-      <formula>AND(NOT(ISBLANK($E165)),$E165&lt;=X$6,$F165&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
+    <cfRule type="expression" dxfId="100" priority="4000">
+      <formula>AND(NOT(ISBLANK($E51)),$E51&lt;=W$6,$F51&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W75:W76">
-    <cfRule type="expression" dxfId="99" priority="4003">
-      <formula>AND(NOT(ISBLANK($E51)),$E51&lt;=W$6,$F51&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="98" priority="4001">
+    <cfRule type="expression" dxfId="99" priority="4001">
       <formula>AND(NOT(ISBLANK($E165)),$E165&lt;=X$6,$F165&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="4002">
+    <cfRule type="expression" dxfId="98" priority="4002">
       <formula>AND($E51&lt;=W$6,ROUNDDOWN(($F51-$E51+1)*$H51,0)+$E51-1&gt;=W$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="97" priority="4003">
+      <formula>AND(NOT(ISBLANK($E51)),$E51&lt;=W$6,$F51&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W77">
@@ -18061,25 +18069,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W81">
-    <cfRule type="expression" dxfId="87" priority="3816">
-      <formula>AND($E67&lt;=W$6,ROUNDDOWN(($F67-$E67+1)*$H67,0)+$E67-1&gt;=W$6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="86" priority="3817">
+    <cfRule type="expression" dxfId="87" priority="3817">
       <formula>AND(NOT(ISBLANK($E67)),$E67&lt;=W$6,$F67&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="3818">
+    <cfRule type="expression" dxfId="86" priority="3818">
       <formula>AND(NOT(ISBLANK($E95)),$E95&lt;=X$6,$F95&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="85" priority="3816">
+      <formula>AND($E67&lt;=W$6,ROUNDDOWN(($F67-$E67+1)*$H67,0)+$E67-1&gt;=W$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W85">
     <cfRule type="expression" dxfId="84" priority="4016">
       <formula>AND($E54&lt;=W$6,ROUNDDOWN(($F54-$E54+1)*$H54,0)+$E54-1&gt;=W$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="4018">
+    <cfRule type="expression" dxfId="83" priority="4017">
+      <formula>AND(NOT(ISBLANK($E54)),$E54&lt;=W$6,$F54&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="82" priority="4018">
       <formula>AND(NOT(ISBLANK($E168)),$E168&lt;=X$6,$F168&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="82" priority="4017">
-      <formula>AND(NOT(ISBLANK($E54)),$E54&lt;=W$6,$F54&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W86">
@@ -18094,14 +18102,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W87:W88">
-    <cfRule type="expression" dxfId="78" priority="4024">
-      <formula>AND(NOT(ISBLANK($E165)),$E165&lt;=X$6,$F165&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
+    <cfRule type="expression" dxfId="78" priority="4022">
+      <formula>AND($E51&lt;=W$6,ROUNDDOWN(($F51-$E51+1)*$H51,0)+$E51-1&gt;=W$6)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="77" priority="4023">
       <formula>AND(NOT(ISBLANK($E51)),$E51&lt;=W$6,$F51&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="4022">
-      <formula>AND($E51&lt;=W$6,ROUNDDOWN(($F51-$E51+1)*$H51,0)+$E51-1&gt;=W$6)</formula>
+    <cfRule type="expression" dxfId="76" priority="4024">
+      <formula>AND(NOT(ISBLANK($E165)),$E165&lt;=X$6,$F165&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W89:W90">
@@ -18147,19 +18155,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W112 W118 W120 W122">
-    <cfRule type="expression" dxfId="65" priority="81">
+    <cfRule type="expression" dxfId="65" priority="82">
+      <formula>AND(NOT(ISBLANK($E110)),$E110&lt;=W$6,$F110&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="64" priority="81">
       <formula>AND($E110&lt;=W$6,ROUNDDOWN(($F110-$E110+1)*$H110,0)+$E110-1&gt;=W$6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="64" priority="82">
-      <formula>AND(NOT(ISBLANK($E110)),$E110&lt;=W$6,$F110&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W125">
-    <cfRule type="expression" dxfId="63" priority="4052">
+    <cfRule type="expression" dxfId="63" priority="4053">
+      <formula>AND(NOT(ISBLANK($E120)),$E120&lt;=W$6,$F120&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="62" priority="4052">
       <formula>AND($E120&lt;=W$6,ROUNDDOWN(($F120-$E120+1)*$H120,0)+$E120-1&gt;=W$6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="62" priority="4053">
-      <formula>AND(NOT(ISBLANK($E120)),$E120&lt;=W$6,$F120&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W126">
@@ -18179,19 +18187,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W129">
-    <cfRule type="expression" dxfId="57" priority="4063">
+    <cfRule type="expression" dxfId="57" priority="4062">
+      <formula>AND($E120&lt;=W$6,ROUNDDOWN(($F120-$E120+1)*$H120,0)+$E120-1&gt;=W$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="56" priority="4063">
       <formula>AND(NOT(ISBLANK($E120)),$E120&lt;=W$6,$F120&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="56" priority="4062">
-      <formula>AND($E120&lt;=W$6,ROUNDDOWN(($F120-$E120+1)*$H120,0)+$E120-1&gt;=W$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W130">
-    <cfRule type="expression" dxfId="55" priority="3698">
+    <cfRule type="expression" dxfId="55" priority="3697">
+      <formula>AND($E125&lt;=W$6,ROUNDDOWN(($F125-$E125+1)*$H125,0)+$E125-1&gt;=W$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="3698">
       <formula>AND(NOT(ISBLANK($E125)),$E125&lt;=W$6,$F125&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="54" priority="3697">
-      <formula>AND($E125&lt;=W$6,ROUNDDOWN(($F125-$E125+1)*$H125,0)+$E125-1&gt;=W$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W131">
@@ -18203,19 +18211,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W132">
-    <cfRule type="expression" dxfId="51" priority="4068">
+    <cfRule type="expression" dxfId="51" priority="4069">
+      <formula>AND(NOT(ISBLANK($E120)),$E120&lt;=W$6,$F120&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="50" priority="4068">
       <formula>AND($E120&lt;=W$6,ROUNDDOWN(($F120-$E120+1)*$H120,0)+$E120-1&gt;=W$6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="50" priority="4069">
-      <formula>AND(NOT(ISBLANK($E120)),$E120&lt;=W$6,$F120&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W133">
-    <cfRule type="expression" dxfId="49" priority="4072">
+    <cfRule type="expression" dxfId="49" priority="4071">
+      <formula>AND($E120&lt;=W$6,ROUNDDOWN(($F120-$E120+1)*$H120,0)+$E120-1&gt;=W$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="4072">
       <formula>AND(NOT(ISBLANK($E120)),$E120&lt;=W$6,$F120&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="48" priority="4071">
-      <formula>AND($E120&lt;=W$6,ROUNDDOWN(($F120-$E120+1)*$H120,0)+$E120-1&gt;=W$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W134">
@@ -18248,11 +18256,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W138">
-    <cfRule type="expression" dxfId="40" priority="4084">
+    <cfRule type="expression" dxfId="40" priority="4083">
+      <formula>AND($E121&lt;=W$6,ROUNDDOWN(($F121-$E121+1)*$H121,0)+$E121-1&gt;=W$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="39" priority="4084">
       <formula>AND(NOT(ISBLANK($E121)),$E121&lt;=W$6,$F121&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="39" priority="4083">
-      <formula>AND($E121&lt;=W$6,ROUNDDOWN(($F121-$E121+1)*$H121,0)+$E121-1&gt;=W$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W139">
@@ -18296,43 +18304,43 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W145">
-    <cfRule type="expression" dxfId="28" priority="4101">
+    <cfRule type="expression" dxfId="28" priority="4102">
+      <formula>AND(NOT(ISBLANK($E122)),$E122&lt;=W$6,$F122&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="4101">
       <formula>AND($E122&lt;=W$6,ROUNDDOWN(($F122-$E122+1)*$H122,0)+$E122-1&gt;=W$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="4102">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W146:W147">
+    <cfRule type="expression" dxfId="26" priority="4104">
+      <formula>AND($E122&lt;=W$6,ROUNDDOWN(($F122-$E122+1)*$H122,0)+$E122-1&gt;=W$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="4105">
       <formula>AND(NOT(ISBLANK($E122)),$E122&lt;=W$6,$F122&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W146:W147">
-    <cfRule type="expression" dxfId="26" priority="4105">
-      <formula>AND(NOT(ISBLANK($E122)),$E122&lt;=W$6,$F122&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
+  <conditionalFormatting sqref="W148">
+    <cfRule type="expression" dxfId="24" priority="4107">
+      <formula>AND($E123&lt;=W$6,ROUNDDOWN(($F123-$E123+1)*$H123,0)+$E123-1&gt;=W$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="4104">
-      <formula>AND($E122&lt;=W$6,ROUNDDOWN(($F122-$E122+1)*$H122,0)+$E122-1&gt;=W$6)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W148">
-    <cfRule type="expression" dxfId="24" priority="4108">
+    <cfRule type="expression" dxfId="23" priority="4108">
       <formula>AND(NOT(ISBLANK($E123)),$E123&lt;=W$6,$F123&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="23" priority="4107">
-      <formula>AND($E123&lt;=W$6,ROUNDDOWN(($F123-$E123+1)*$H123,0)+$E123-1&gt;=W$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W149">
-    <cfRule type="expression" dxfId="22" priority="4111">
+    <cfRule type="expression" dxfId="22" priority="4110">
+      <formula>AND($E123&lt;=W$6,ROUNDDOWN(($F123-$E123+1)*$H123,0)+$E123-1&gt;=W$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="4111">
       <formula>AND(NOT(ISBLANK($E123)),$E123&lt;=W$6,$F123&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="21" priority="4110">
-      <formula>AND($E123&lt;=W$6,ROUNDDOWN(($F123-$E123+1)*$H123,0)+$E123-1&gt;=W$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W150:W151 W153:W155">
-    <cfRule type="expression" dxfId="20" priority="4113">
+    <cfRule type="expression" dxfId="20" priority="4112">
+      <formula>AND($E120&lt;=W$6,ROUNDDOWN(($F120-$E120+1)*$H120,0)+$E120-1&gt;=W$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="4113">
       <formula>AND(NOT(ISBLANK($E120)),$E120&lt;=W$6,$F120&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="4112">
-      <formula>AND($E120&lt;=W$6,ROUNDDOWN(($F120-$E120+1)*$H120,0)+$E120-1&gt;=W$6)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="18" priority="4114">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=X$6,#REF!&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
@@ -18347,11 +18355,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W156">
-    <cfRule type="expression" dxfId="15" priority="4119">
+    <cfRule type="expression" dxfId="15" priority="4118">
+      <formula>AND($E125&lt;=W$6,ROUNDDOWN(($F125-$E125+1)*$H125,0)+$E125-1&gt;=W$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="4119">
       <formula>AND(NOT(ISBLANK($E125)),$E125&lt;=W$6,$F125&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="4118">
-      <formula>AND($E125&lt;=W$6,ROUNDDOWN(($F125-$E125+1)*$H125,0)+$E125-1&gt;=W$6)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="13" priority="4120">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=X$6,#REF!&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
@@ -18369,11 +18377,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W158:W159">
-    <cfRule type="expression" dxfId="9" priority="9">
+    <cfRule type="expression" dxfId="9" priority="8">
+      <formula>AND($E122&lt;=W$6,ROUNDDOWN(($F122-$E122+1)*$H122,0)+$E122-1&gt;=W$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>AND(NOT(ISBLANK($E122)),$E122&lt;=W$6,$F122&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="8">
-      <formula>AND($E122&lt;=W$6,ROUNDDOWN(($F122-$E122+1)*$H122,0)+$E122-1&gt;=W$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W158:W161">
@@ -18382,30 +18390,30 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W160:W161">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="6" priority="6">
+      <formula>AND($E122&lt;=W$6,ROUNDDOWN(($F122-$E122+1)*$H122,0)+$E122-1&gt;=W$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>AND(NOT(ISBLANK($E122)),$E122&lt;=W$6,$F122&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="6">
-      <formula>AND($E122&lt;=W$6,ROUNDDOWN(($F122-$E122+1)*$H122,0)+$E122-1&gt;=W$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W162">
-    <cfRule type="expression" dxfId="4" priority="4126">
-      <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=X$6,#REF!&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="4124">
+    <cfRule type="expression" dxfId="4" priority="4124">
       <formula>AND($E123&lt;=W$6,ROUNDDOWN(($F123-$E123+1)*$H123,0)+$E123-1&gt;=W$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4125">
+    <cfRule type="expression" dxfId="3" priority="4125">
       <formula>AND(NOT(ISBLANK($E123)),$E123&lt;=W$6,$F123&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="4126">
+      <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=X$6,#REF!&gt;=X$6,WEEKDAY(X$6,2)&gt;=6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W163">
-    <cfRule type="expression" dxfId="1" priority="1513">
+    <cfRule type="expression" dxfId="1" priority="1512">
+      <formula>AND($E105&lt;=W$6,ROUNDDOWN(($F105-$E105+1)*$H105,0)+$E105-1&gt;=W$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="1513">
       <formula>AND(NOT(ISBLANK($E105)),$E105&lt;=W$6,$F105&gt;=W$6,WEEKDAY(W$6,2)&lt;=5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="1512">
-      <formula>AND($E105&lt;=W$6,ROUNDDOWN(($F105-$E105+1)*$H105,0)+$E105-1&gt;=W$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0" footer="0"/>

</xml_diff>